<commit_message>
bulk final version, going to be optimized
</commit_message>
<xml_diff>
--- a/result/10-4_vicuna13-vip_nonvis-optim_500/eval/scoring_template.xlsx
+++ b/result/10-4_vicuna13-vip_nonvis-optim_500/eval/scoring_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="377">
   <si>
     <t>rules</t>
   </si>
@@ -305,442 +305,910 @@
     <t>reasoned_answer</t>
   </si>
   <si>
+    <t>2345458.jpg</t>
+  </si>
+  <si>
+    <t>2408290.jpg</t>
+  </si>
+  <si>
+    <t>2321389.jpg</t>
+  </si>
+  <si>
+    <t>2380438.jpg</t>
+  </si>
+  <si>
+    <t>1159351.jpg</t>
+  </si>
+  <si>
+    <t>2403286.jpg</t>
+  </si>
+  <si>
+    <t>2335580.jpg</t>
+  </si>
+  <si>
+    <t>2387492.jpg</t>
+  </si>
+  <si>
+    <t>2347921.jpg</t>
+  </si>
+  <si>
+    <t>2353575.jpg</t>
+  </si>
+  <si>
+    <t>2342596.jpg</t>
+  </si>
+  <si>
+    <t>2402093.jpg</t>
+  </si>
+  <si>
+    <t>2320752.jpg</t>
+  </si>
+  <si>
+    <t>2356501.jpg</t>
+  </si>
+  <si>
+    <t>2394235.jpg</t>
+  </si>
+  <si>
+    <t>2384295.jpg</t>
+  </si>
+  <si>
+    <t>2329535.jpg</t>
+  </si>
+  <si>
     <t>2321990.jpg</t>
   </si>
   <si>
-    <t>2403286.jpg</t>
-  </si>
-  <si>
-    <t>2402093.jpg</t>
-  </si>
-  <si>
-    <t>2380438.jpg</t>
+    <t>2366289.jpg</t>
+  </si>
+  <si>
+    <t>2361750.jpg</t>
   </si>
   <si>
     <t>2360023.jpg</t>
   </si>
   <si>
+    <t>2393668.jpg</t>
+  </si>
+  <si>
+    <t>2417032.jpg</t>
+  </si>
+  <si>
+    <t>2341916.jpg</t>
+  </si>
+  <si>
+    <t>2387659.jpg</t>
+  </si>
+  <si>
+    <t>2324496.jpg</t>
+  </si>
+  <si>
+    <t>2338295.jpg</t>
+  </si>
+  <si>
     <t>2378845.jpg</t>
   </si>
   <si>
-    <t>2361750.jpg</t>
-  </si>
-  <si>
-    <t>2342596.jpg</t>
-  </si>
-  <si>
-    <t>2384295.jpg</t>
+    <t>2404643.jpg</t>
+  </si>
+  <si>
+    <t>2417850.jpg</t>
   </si>
   <si>
     <t>2349840.jpg</t>
   </si>
   <si>
-    <t>2404643.jpg</t>
-  </si>
-  <si>
-    <t>2347921.jpg</t>
-  </si>
-  <si>
-    <t>2356501.jpg</t>
-  </si>
-  <si>
-    <t>2353575.jpg</t>
-  </si>
-  <si>
-    <t>1159351.jpg</t>
-  </si>
-  <si>
-    <t>2341916.jpg</t>
-  </si>
-  <si>
-    <t>2335580.jpg</t>
+    <t>2328035.jpg</t>
+  </si>
+  <si>
+    <t>2335961.jpg</t>
+  </si>
+  <si>
+    <t>2402695.jpg</t>
+  </si>
+  <si>
+    <t>2340260.jpg</t>
+  </si>
+  <si>
+    <t>Is the man wearing jeans?</t>
+  </si>
+  <si>
+    <t>What is the purpose of the wheel in a motorcycle?</t>
+  </si>
+  <si>
+    <t>What is the color of the snow in the image?</t>
+  </si>
+  <si>
+    <t>Is the shirt worn by the man on the left side of the image?</t>
+  </si>
+  <si>
+    <t>What is the man's name?</t>
+  </si>
+  <si>
+    <t>What type of food is on the plate?</t>
+  </si>
+  <si>
+    <t>Where is the child located?</t>
+  </si>
+  <si>
+    <t>Is the building in the background a commercial establishment?</t>
+  </si>
+  <si>
+    <t>What is the purpose of the sign with the red mask contour?</t>
+  </si>
+  <si>
+    <t>Is the boy standing in the grass?</t>
+  </si>
+  <si>
+    <t>Is the street wet?</t>
+  </si>
+  <si>
+    <t>How many rays of sunlight are visible in the image?</t>
+  </si>
+  <si>
+    <t>What is the architectural style of the building?</t>
+  </si>
+  <si>
+    <t>What is the man's role in the tennis event?</t>
+  </si>
+  <si>
+    <t>How many leaves are visible in the image?</t>
+  </si>
+  <si>
+    <t>What is the boy's name?</t>
+  </si>
+  <si>
+    <t>What is the color of the vase holding the bouquet?</t>
+  </si>
+  <si>
+    <t>What is the color of the desk in the image?</t>
+  </si>
+  <si>
+    <t>What is the color of the cat in the image?</t>
+  </si>
+  <si>
+    <t>Is the sky clear?</t>
+  </si>
+  <si>
+    <t>Which table is closest to the camera?</t>
+  </si>
+  <si>
+    <t>What type of bush is this?</t>
+  </si>
+  <si>
+    <t>What is the name of the mountain in the background of the image?</t>
+  </si>
+  <si>
+    <t>Is the man in the image holding a video game controller?</t>
+  </si>
+  <si>
+    <t>What is the color of the sky in the image?</t>
+  </si>
+  <si>
+    <t>What is the purpose of the windshield on a train?</t>
+  </si>
+  <si>
+    <t>How many airplanes are visible in the image?</t>
+  </si>
+  <si>
+    <t>How many slices of pizza are on the plate?</t>
+  </si>
+  <si>
+    <t>What is the time displayed on the clock?</t>
+  </si>
+  <si>
+    <t>How many people are in the image?</t>
+  </si>
+  <si>
+    <t>Which man is wearing glasses?</t>
+  </si>
+  <si>
+    <t>Is the spoon in the pot of rice?</t>
+  </si>
+  <si>
+    <t>What type of attire is the man wearing in the image?</t>
+  </si>
+  <si>
+    <t>What is the color of the bike in the image?</t>
+  </si>
+  <si>
+    <t>How many pillows are on the bed?</t>
+  </si>
+  <si>
+    <t>What is the primary food source for giraffes in their natural habitat?</t>
+  </si>
+  <si>
+    <t>What is the color of the shirt the person is wearing?</t>
+  </si>
+  <si>
+    <t>Is the faucet in the sink?</t>
+  </si>
+  <si>
+    <t>Which racket is being held by the person in the image?</t>
+  </si>
+  <si>
+    <t>Is the pot on the step?</t>
+  </si>
+  <si>
+    <t>Is the grass in the image green?</t>
+  </si>
+  <si>
+    <t>What type of food is being cooked in the pot within the red rectangle?</t>
+  </si>
+  <si>
+    <t>What is the name of the building with the sign that says 'Arts &amp; Entertainment Hustle'?</t>
+  </si>
+  <si>
+    <t>Where is the bench located?</t>
+  </si>
+  <si>
+    <t>What is the color of the car in the image?</t>
   </si>
   <si>
     <t>Is the bandana on the cat?</t>
   </si>
   <si>
-    <t>What type of food is on the plate?</t>
-  </si>
-  <si>
-    <t>How many rays of sunlight are visible in the image?</t>
-  </si>
-  <si>
-    <t>Is the shirt worn by the man on the left side of the image?</t>
+    <t>What is the purpose of the hair on the animal's head?</t>
+  </si>
+  <si>
+    <t>Is the hair of the boy short?</t>
   </si>
   <si>
     <t>What is the condition of the ground in the image?</t>
   </si>
   <si>
+    <t>What color are the cars of the train?</t>
+  </si>
+  <si>
+    <t>What is the color of the man's hair?</t>
+  </si>
+  <si>
+    <t>Which rose has a lighter color with a darker center?</t>
+  </si>
+  <si>
+    <t>What is the color of the door?</t>
+  </si>
+  <si>
+    <t>What is the tree in the background?</t>
+  </si>
+  <si>
+    <t>Where is the tree located in relation to the train tracks?</t>
+  </si>
+  <si>
+    <t>Is the tree in the image healthy?</t>
+  </si>
+  <si>
+    <t>How many people are visible in the mirror?</t>
+  </si>
+  <si>
+    <t>What is the color of the water in the image?</t>
+  </si>
+  <si>
+    <t>Is the machine in the background turned on?</t>
+  </si>
+  <si>
+    <t>What is the condition of the wall behind the sink?</t>
+  </si>
+  <si>
+    <t>How many hairs are in the man's beard?</t>
+  </si>
+  <si>
+    <t>How many shirts are visible in the image?</t>
+  </si>
+  <si>
+    <t>Where are the clouds in the sky?</t>
+  </si>
+  <si>
+    <t>What is the location of the green and red train in the image?</t>
+  </si>
+  <si>
+    <t>What type of vest is the man wearing?</t>
+  </si>
+  <si>
+    <t>What is the name of the garage in the image?</t>
+  </si>
+  <si>
+    <t>How many types of sauce are visible on the plate?</t>
+  </si>
+  <si>
+    <t>Is the hair of the horse visible?</t>
+  </si>
+  <si>
     <t>What is the condition of the floor in the image?</t>
   </si>
   <si>
-    <t>What is the name of the mountain in the background of the image?</t>
-  </si>
-  <si>
-    <t>What is the color of the sky in the image?</t>
+    <t>What is the man's occupation?</t>
+  </si>
+  <si>
+    <t>Is the jacket worn by the police officer in the image?</t>
+  </si>
+  <si>
+    <t>What is the altitude of the snowy mountain range in the background?</t>
   </si>
   <si>
     <t>What is the purpose of the steps in the image?</t>
   </si>
   <si>
-    <t>What is the name of the building with the sign that says 'Arts &amp; Entertainment Hustle'?</t>
-  </si>
-  <si>
-    <t>What is the color of the cat in the image?</t>
-  </si>
-  <si>
-    <t>What is the boy's name?</t>
-  </si>
-  <si>
-    <t>What is the color of the man's hair?</t>
-  </si>
-  <si>
-    <t>Is the hair of the boy short?</t>
-  </si>
-  <si>
-    <t>What is the color of the door?</t>
-  </si>
-  <si>
-    <t>How many types of sauce are visible on the plate?</t>
-  </si>
-  <si>
-    <t>How many shirts are visible in the image?</t>
-  </si>
-  <si>
-    <t>Which man is wearing glasses?</t>
-  </si>
-  <si>
-    <t>What is the purpose of the windshield on a train?</t>
-  </si>
-  <si>
-    <t>How many slices of pizza are on the plate?</t>
-  </si>
-  <si>
-    <t>What is the purpose of the hair on the animal's head?</t>
-  </si>
-  <si>
-    <t>Which racket is being held by the person in the image?</t>
-  </si>
-  <si>
-    <t>Is the sky clear?</t>
-  </si>
-  <si>
-    <t>Is the boy standing in the grass?</t>
-  </si>
-  <si>
-    <t>What is the man's name?</t>
-  </si>
-  <si>
-    <t>What type of food is being cooked in the pot within the red rectangle?</t>
-  </si>
-  <si>
-    <t>What is the man's role in the tennis event?</t>
-  </si>
-  <si>
-    <t>What is the color of the bike in the image?</t>
+    <t>Is the building in the background part of the airport's infrastructure?</t>
+  </si>
+  <si>
+    <t>How many men are visible in the image?</t>
+  </si>
+  <si>
+    <t>How many giraffes are visible in the image?</t>
+  </si>
+  <si>
+    <t>What type of cloud is in the sky?</t>
   </si>
   <si>
     <t>Is the oil in the pan hot enough to cook the fish?</t>
   </si>
   <si>
-    <t>How many people are in the image?</t>
-  </si>
-  <si>
-    <t>Where is the tree located in relation to the train tracks?</t>
-  </si>
-  <si>
     <t>How many pairs of shorts are visible in the image?</t>
   </si>
   <si>
+    <t>How many wheels does the bike have?</t>
+  </si>
+  <si>
     <t>What is the hair color of the girl in the image?</t>
   </si>
   <si>
     <t>What is the man doing in the image?</t>
   </si>
   <si>
-    <t>Is the machine in the background turned on?</t>
-  </si>
-  <si>
-    <t>What is the color of the shirt the person is wearing?</t>
-  </si>
-  <si>
     <t>Is the ground covered with grass?</t>
   </si>
   <si>
-    <t>What is the purpose of the sign with the red mask contour?</t>
-  </si>
-  <si>
-    <t>Where is the child located?</t>
-  </si>
-  <si>
-    <t>Is the street wet?</t>
-  </si>
-  <si>
-    <t>Is the faucet in the sink?</t>
+    <t>Is the mound on the mountain a natural formation or a man-made structure?</t>
+  </si>
+  <si>
+    <t>What is the man's attire?</t>
+  </si>
+  <si>
+    <t>Is the person in the image skiing down a snowy mountain?</t>
+  </si>
+  <si>
+    <t>What is the snow covering the ground?</t>
+  </si>
+  <si>
+    <t>How many mountains are visible in the background?</t>
   </si>
   <si>
     <t>Is the umbrella open?</t>
   </si>
   <si>
-    <t>Is the pot on the step?</t>
-  </si>
-  <si>
-    <t>Is the man in the image holding a video game controller?</t>
+    <t>What color is the train car in the image?</t>
+  </si>
+  <si>
+    <t>Is there a variety of carrots on the table?</t>
   </si>
   <si>
     <t>How many magazines are on the table?</t>
   </si>
   <si>
-    <t>Is the spoon in the pot of rice?</t>
-  </si>
-  <si>
-    <t>What color are the cars of the train?</t>
+    <t>How many players are on the tennis court?</t>
+  </si>
+  <si>
+    <t>How many people are riding the motorcycle?</t>
+  </si>
+  <si>
+    <t>No, the man is not wearing jeans.</t>
+  </si>
+  <si>
+    <t>The wheel provides traction and allows the motorcycle to move.</t>
+  </si>
+  <si>
+    <t>The snow in the image is white.</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
+    <t>The man's name is not visible in the image.</t>
+  </si>
+  <si>
     <t>Mexican cuisine</t>
   </si>
   <si>
+    <t>The child is located in a grassy field.</t>
+  </si>
+  <si>
+    <t>Yes, it appears to be a storefront.</t>
+  </si>
+  <si>
+    <t>The sign with the red mask contour is there to inform people that smoking is not allowed in that area.</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
+    <t>Gothic Revival</t>
+  </si>
+  <si>
+    <t>He is a ball boy.</t>
+  </si>
+  <si>
+    <t>There are hundreds of leaves visible in the image.</t>
+  </si>
+  <si>
+    <t>The boy's name is not visible in the image.</t>
+  </si>
+  <si>
+    <t>The vase is purple.</t>
+  </si>
+  <si>
+    <t>The desk in the image is brown.</t>
+  </si>
+  <si>
+    <t>The cat is black.</t>
+  </si>
+  <si>
+    <t>The table on the far left.</t>
+  </si>
+  <si>
+    <t>It appears to be a green bush with small leaves.</t>
+  </si>
+  <si>
+    <t>It is not possible to determine the name of the mountain from the image alone.</t>
+  </si>
+  <si>
+    <t>Yes, the man is holding a video game controller.</t>
+  </si>
+  <si>
+    <t>The sky in the image is blue.</t>
+  </si>
+  <si>
+    <t>The windshield on a train serves as a window for the train operator to see the tracks ahead and the surroundings.</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>11:25</t>
+  </si>
+  <si>
+    <t>The man on the left.</t>
+  </si>
+  <si>
+    <t>The man is wearing a light-colored suit with a tie.</t>
+  </si>
+  <si>
+    <t>The bike in the image is yellow.</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Giraffes primarily feed on leaves, flowers, and fruits from trees and shrubs, with the acacia tree being one of their favorites.</t>
+  </si>
+  <si>
+    <t>The shirt is blue.</t>
+  </si>
+  <si>
+    <t>The sky in the image is orange.</t>
+  </si>
+  <si>
+    <t>The racket being held is a tennis racket.</t>
+  </si>
+  <si>
+    <t>Yes, the grass in the image is green.</t>
+  </si>
+  <si>
+    <t>Onions are being cooked in the pot within the red rectangle.</t>
+  </si>
+  <si>
+    <t>The building with the sign that says 'Arts &amp; Entertainment Hustle' is called the 'Arts &amp; Entertainment Hustle'.</t>
+  </si>
+  <si>
+    <t>It is located on the sidewalk.</t>
+  </si>
+  <si>
+    <t>The car in the image is green.</t>
+  </si>
+  <si>
+    <t>Insulation and protection from the elements.</t>
+  </si>
+  <si>
     <t>The ground appears to be rocky and uneven.</t>
   </si>
   <si>
+    <t>The cars of the train are blue.</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>The rose in the middle of the bouquet.</t>
+  </si>
+  <si>
+    <t>The door is brown.</t>
+  </si>
+  <si>
+    <t>It is a giraffe.</t>
+  </si>
+  <si>
+    <t>The tree is located beside the train tracks.</t>
+  </si>
+  <si>
+    <t>No, the tree appears to be dead.</t>
+  </si>
+  <si>
+    <t>The table in the foreground.</t>
+  </si>
+  <si>
+    <t>The water in the image is blue.</t>
+  </si>
+  <si>
+    <t>The wall is in poor condition, with visible peeling paint and damage.</t>
+  </si>
+  <si>
+    <t>Many</t>
+  </si>
+  <si>
+    <t>The clouds are in the sky above the trees.</t>
+  </si>
+  <si>
+    <t>The train is located on the tracks in a rural area.</t>
+  </si>
+  <si>
+    <t>He is wearing a black vest.</t>
+  </si>
+  <si>
+    <t>The name of the garage is Orlandi's Tire &amp; Auto Service.</t>
+  </si>
+  <si>
+    <t>Yes, the horse has brown hair.</t>
+  </si>
+  <si>
     <t>The floor appears to be in poor condition, with visible signs of wear and damage.</t>
   </si>
   <si>
-    <t>It is not possible to determine the name of the mountain from the image alone.</t>
-  </si>
-  <si>
-    <t>The sky in the image is blue.</t>
+    <t>He is a businessman.</t>
+  </si>
+  <si>
+    <t>Yes, the jacket is worn by the police officer.</t>
+  </si>
+  <si>
+    <t>The altitude is high, likely above 10,000 feet.</t>
   </si>
   <si>
     <t>The steps in the image likely serve as a means of access to the building above.</t>
   </si>
   <si>
-    <t>The building with the sign that says 'Arts &amp; Entertainment Hustle' is called the 'Arts &amp; Entertainment Hustle'.</t>
-  </si>
-  <si>
-    <t>The cat is black.</t>
-  </si>
-  <si>
-    <t>The boy's name is not visible in the image.</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>The door is brown.</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>The man on the left.</t>
-  </si>
-  <si>
-    <t>The windshield on a train serves as a window for the train operator to see the tracks ahead and the surroundings.</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>The sky in the image is orange.</t>
-  </si>
-  <si>
-    <t>Insulation and protection from the elements.</t>
-  </si>
-  <si>
-    <t>The racket being held is a tennis racket.</t>
-  </si>
-  <si>
-    <t>The man's name is not visible in the image.</t>
-  </si>
-  <si>
-    <t>Onions are being cooked in the pot within the red rectangle.</t>
-  </si>
-  <si>
-    <t>He is a ball boy.</t>
-  </si>
-  <si>
-    <t>The bike in the image is yellow.</t>
+    <t>Yes, the building is part of the airport's infrastructure.</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>There are three giraffes visible in the image.</t>
+  </si>
+  <si>
+    <t>Cumulus cloud</t>
   </si>
   <si>
     <t>Yes, the oil appears to be hot enough to cook the fish.</t>
   </si>
   <si>
-    <t>The tree is located beside the train tracks.</t>
-  </si>
-  <si>
     <t>The man appears to be standing on the grass.</t>
   </si>
   <si>
-    <t>The shirt is blue.</t>
-  </si>
-  <si>
-    <t>The sign with the red mask contour is there to inform people that smoking is not allowed in that area.</t>
-  </si>
-  <si>
-    <t>The child is located in a grassy field.</t>
-  </si>
-  <si>
-    <t>Yes, the man is holding a video game controller.</t>
-  </si>
-  <si>
-    <t>The cars of the train are blue.</t>
+    <t>The mound is a natural formation, likely created by weathering and erosion processes.</t>
+  </si>
+  <si>
+    <t>The man is wearing a light blue shirt, a dark blue tie, and light-colored pants.</t>
+  </si>
+  <si>
+    <t>Yes, the person is skiing down a snowy mountain.</t>
+  </si>
+  <si>
+    <t>The snow is covering the ground because it has fallen from the sky.</t>
+  </si>
+  <si>
+    <t>The train car in the image is green.</t>
+  </si>
+  <si>
+    <t>Yes, there are different types of carrots on the table.</t>
+  </si>
+  <si>
+    <t>The man is wearing a pair of dark-colored pants that are not denim.</t>
+  </si>
+  <si>
+    <t>The wheel is a crucial component of a motorcycle as it allows the vehicle to move by providing traction on the road surface.</t>
+  </si>
+  <si>
+    <t>The snow appears to be white, which is the typical color for snow when it is fresh and has not been disturbed.</t>
+  </si>
+  <si>
+    <t>The shirt is visible on the man's body and is part of his attire.</t>
+  </si>
+  <si>
+    <t>The image only shows the back of the man's head and his clothing, which does not provide any information about his name.</t>
+  </si>
+  <si>
+    <t>The plate contains rice, beans, and what appears to be a type of meat covered in a green sauce, which are common ingredients in Mexican dishes.</t>
+  </si>
+  <si>
+    <t>The child is surrounded by grass and there are no visible structures or landmarks in the background, indicating an outdoor, open space.</t>
+  </si>
+  <si>
+    <t>The signage and the presence of a bench in front suggest it is a place where people can sit and possibly shop.</t>
+  </si>
+  <si>
+    <t>The sign with the red mask contour is typically used to communicate rules or regulations to the public, and in this case, it is indicating that smoking is prohibited in that particular space.</t>
+  </si>
+  <si>
+    <t>The boy is standing on the grass, which is a natural outdoor surface.</t>
+  </si>
+  <si>
+    <t>The street appears to be wet, likely due to recent rain.</t>
+  </si>
+  <si>
+    <t>There is only one ray of sunlight visible in the image, which is the one that is casting the shadow of the skateboarder.</t>
+  </si>
+  <si>
+    <t>The building features pointed arches, ornate detailing, and a clock face with Roman numerals, which are characteristic of Gothic Revival architecture.</t>
+  </si>
+  <si>
+    <t>He is wearing a ball boy uniform and is holding a basket of tennis balls.</t>
+  </si>
+  <si>
+    <t>The image shows a dense forest with a variety of trees and shrubs, all of which have leaves.</t>
+  </si>
+  <si>
+    <t>The boy's name is not written on his shirt or any other part of his clothing that is visible in the image.</t>
+  </si>
+  <si>
+    <t>The vase is made of a material that reflects light and appears purple.</t>
+  </si>
+  <si>
+    <t>The desk appears to have a light brown color, which is commonly associated with wood.</t>
+  </si>
+  <si>
+    <t>The cat has a solid black fur coat.</t>
+  </si>
+  <si>
+    <t>There are no visible clouds in the sky.</t>
+  </si>
+  <si>
+    <t>The table is positioned in such a way that it is the first one that would be seen by someone looking at the camera.</t>
+  </si>
+  <si>
+    <t>The leaves are a deep green color and seem to be small and round in shape, which is typical of certain types of bushes.</t>
+  </si>
+  <si>
+    <t>The mountain is not labeled or identified with any specific name or location.</t>
+  </si>
+  <si>
+    <t>The man is holding a device that resembles a video game controller, which is commonly used to interact with video games.</t>
+  </si>
+  <si>
+    <t>The sky appears to be clear and bright, which suggests it is daytime, and the color appears to be a vibrant blue.</t>
+  </si>
+  <si>
+    <t>The windshield is a crucial part of the train's design, providing visibility for the operator to navigate the train safely.</t>
+  </si>
+  <si>
+    <t>The plate contains a dish with melted cheese, beans, and rice, which are common ingredients in Mexican food.</t>
+  </si>
+  <si>
+    <t>There is only one airplane visible in the image, which is a large commercial jet.</t>
+  </si>
+  <si>
+    <t>There are three slices of pizza on the plate.</t>
+  </si>
+  <si>
+    <t>The clock shows the hands on the numbers 11 and 25, indicating that the time is 11:25.</t>
+  </si>
+  <si>
+    <t>There are three people in the image, one is a young boy eating pizza, another is a man in a white shirt standing behind him, and the third is a woman sitting at a table in the background.</t>
+  </si>
+  <si>
+    <t>The man on the left is wearing glasses, while the man on the right is not.</t>
+  </si>
+  <si>
+    <t>The sky appears to be clear and cloudless, which is typical for a bright blue sky.</t>
+  </si>
+  <si>
+    <t>The spoon is partially submerged in the pot of rice, indicating it is being used to stir the rice.</t>
+  </si>
+  <si>
+    <t>The man is dressed in a formal manner, which is appropriate for a tennis match or event.</t>
+  </si>
+  <si>
+    <t>The bike has a bright yellow frame which is visible in the image.</t>
+  </si>
+  <si>
+    <t>There are two pillows on the bed, one yellow and one white.</t>
+  </si>
+  <si>
+    <t>Giraffes have a specialized diet that allows them to access food sources that are out of reach for many other herbivores. Their long necks and legs enable them to browse on foliage that is high up in the trees, giving them a competitive advantage in their ecosystem.</t>
+  </si>
+  <si>
+    <t>The shirt appears to be blue in color.</t>
+  </si>
+  <si>
+    <t>The sky appears to have a warm orange hue, which is often associated with sunset or sunrise.</t>
+  </si>
+  <si>
+    <t>The faucet is attached to the sink and is part of the sink's fixtures.</t>
+  </si>
+  <si>
+    <t>The racket has a tightly woven mesh pattern and is designed for hitting a tennis ball, which is typical of tennis rackets.</t>
+  </si>
+  <si>
+    <t>The pot is placed on the step, which is part of the staircase.</t>
+  </si>
+  <si>
+    <t>The grass appears to be healthy and vibrant, which is typical for green grass.</t>
+  </si>
+  <si>
+    <t>The pot within the red rectangle contains sliced onions that are submerged in liquid, which is a common way to cook onions.</t>
+  </si>
+  <si>
+    <t>The sign on the building indicates that it is called the 'Arts &amp; Entertainment Hustle'.</t>
+  </si>
+  <si>
+    <t>The bench is positioned on the sidewalk, which is a common place for such seating furniture.</t>
+  </si>
+  <si>
+    <t>The sky appears to be clear and bright, which is typical for a daytime scene, and the color blue is often associated with clear skies.</t>
+  </si>
+  <si>
+    <t>The car has a predominantly green color with some red and white accents.</t>
   </si>
   <si>
     <t>The bandana is tied around the cat's neck.</t>
   </si>
   <si>
-    <t>The plate contains rice, beans, and what appears to be a type of meat covered in a green sauce, which are common ingredients in Mexican dishes.</t>
-  </si>
-  <si>
-    <t>There is only one ray of sunlight visible in the image, which is the one that is casting the shadow of the skateboarder.</t>
-  </si>
-  <si>
-    <t>The shirt is visible on the man's body and is part of his attire.</t>
+    <t>The long, thick hair on the animal's head helps to insulate its body heat and protect it from harsh weather conditions such as cold winds and rain.</t>
+  </si>
+  <si>
+    <t>The hair of the boy is neatly trimmed and does not appear to be long.</t>
   </si>
   <si>
     <t>The ground is covered with a mix of rocks and dirt, which suggests that it is not a smooth surface.</t>
   </si>
   <si>
+    <t>The cars of the train are painted in a bright blue color, which is a common color for train cars.</t>
+  </si>
+  <si>
+    <t>The man's hair appears to be of a dark brown color.</t>
+  </si>
+  <si>
+    <t>The rose in the middle has a lighter color with a darker center, which is typical of roses that have been cut and are no longer receiving sunlight.</t>
+  </si>
+  <si>
+    <t>The door has a wooden frame and a brown color which is typical for wooden doors.</t>
+  </si>
+  <si>
+    <t>The tree is tall with a long neck, which is characteristic of a giraffe.</t>
+  </si>
+  <si>
+    <t>The tree is positioned alongside the railroad tracks, indicating that it is adjacent to the tracks.</t>
+  </si>
+  <si>
+    <t>The tree has no leaves and its branches are bare, indicating that it is not alive.</t>
+  </si>
+  <si>
+    <t>The table is in the foreground and is the closest to the camera.</t>
+  </si>
+  <si>
+    <t>The reflection in the mirror shows a single individual.</t>
+  </si>
+  <si>
+    <t>The water appears to be a deep blue color, which is typical for open ocean water.</t>
+  </si>
+  <si>
+    <t>The machine has lights on and appears to be in use.</t>
+  </si>
+  <si>
+    <t>The peeling paint and the exposed pipes suggest that the wall has been neglected and is in need of repair or renovation.</t>
+  </si>
+  <si>
+    <t>The man has a thick beard with a lot of hairs.</t>
+  </si>
+  <si>
+    <t>There are two men in the image, and both are wearing shirts.</t>
+  </si>
+  <si>
+    <t>The clouds are visible in the sky and they are above the trees, indicating that they are at a higher altitude than the trees.</t>
+  </si>
+  <si>
+    <t>The train is surrounded by open fields and there are no urban structures visible in the background, indicating a rural setting.</t>
+  </si>
+  <si>
+    <t>The vest is black in color and appears to be a formal or semi-formal garment.</t>
+  </si>
+  <si>
+    <t>The name of the garage is visible on the sign above the door.</t>
+  </si>
+  <si>
+    <t>There is a yellow sauce and a green sauce on the plate.</t>
+  </si>
+  <si>
+    <t>The horse's hair is clearly visible and it appears to be brown in color.</t>
+  </si>
+  <si>
     <t>The floor has chipped paint, rust stains, and what looks like water damage, indicating it has not been well-maintained.</t>
   </si>
   <si>
-    <t>The mountain is not labeled or identified with any specific name or location.</t>
-  </si>
-  <si>
-    <t>The sky appears to be clear and bright, which is typical for a daytime scene, and the color blue is often associated with clear skies.</t>
+    <t>He is wearing a dress shirt and tie, which is typical attire for a professional setting.</t>
+  </si>
+  <si>
+    <t>The jacket is part of the uniform that the police officer is wearing.</t>
+  </si>
+  <si>
+    <t>The snow is thick and the peaks are jagged, indicating a high altitude where the air is thinner and colder.</t>
   </si>
   <si>
     <t>Steps are typically used to provide a safe and convenient way for pedestrians to reach higher levels, such as the building in the background.</t>
   </si>
   <si>
-    <t>The sign on the building indicates that it is called the 'Arts &amp; Entertainment Hustle'.</t>
-  </si>
-  <si>
-    <t>The cat has a solid black fur coat.</t>
-  </si>
-  <si>
-    <t>The boy's name is not written on his shirt or any other part of his clothing that is visible in the image.</t>
+    <t>The building is located within the airport's premises and is likely used for airport operations.</t>
+  </si>
+  <si>
+    <t>There are four men in the image, all of whom are wearing uniforms and appear to be police officers.</t>
+  </si>
+  <si>
+    <t>The image shows three giraffes standing in a row, with one of them appearing to be in motion.</t>
+  </si>
+  <si>
+    <t>Cumulus clouds are fluffy and white, and they often have a flat base.</t>
   </si>
   <si>
     <t>The sky appears to be clear and cloudless, which is typical for a blue sky.</t>
   </si>
   <si>
-    <t>The man's hair appears to be of a dark brown color.</t>
-  </si>
-  <si>
-    <t>The hair of the boy is neatly trimmed and does not appear to be long.</t>
-  </si>
-  <si>
-    <t>The door has a wooden frame and a brown color which is typical for wooden doors.</t>
-  </si>
-  <si>
-    <t>There is a yellow sauce and a green sauce on the plate.</t>
-  </si>
-  <si>
-    <t>There are two men in the image, and both are wearing shirts.</t>
-  </si>
-  <si>
-    <t>The man on the left is wearing glasses, while the man on the right is not.</t>
-  </si>
-  <si>
-    <t>The windshield is a crucial part of the train's design, providing visibility for the operator to navigate the train safely.</t>
-  </si>
-  <si>
-    <t>There are three slices of pizza on the plate.</t>
-  </si>
-  <si>
-    <t>The sky appears to have a warm orange hue, which is often associated with sunset or sunrise.</t>
-  </si>
-  <si>
-    <t>The long, thick hair on the animal's head helps to insulate its body heat and protect it from harsh weather conditions such as cold winds and rain.</t>
-  </si>
-  <si>
-    <t>The racket has a tightly woven mesh pattern and is designed for hitting a tennis ball, which is typical of tennis rackets.</t>
-  </si>
-  <si>
-    <t>There are no visible clouds in the sky.</t>
-  </si>
-  <si>
-    <t>The boy is standing on the grass, which is a natural outdoor surface.</t>
-  </si>
-  <si>
-    <t>The image only shows the back of the man's head and his clothing, which does not provide any information about his name.</t>
-  </si>
-  <si>
-    <t>The pot within the red rectangle contains sliced onions that are submerged in liquid, which is a common way to cook onions.</t>
-  </si>
-  <si>
-    <t>He is wearing a ball boy uniform and is holding a basket of tennis balls.</t>
-  </si>
-  <si>
-    <t>The bike has a bright yellow frame which is visible in the image.</t>
-  </si>
-  <si>
     <t>The oil is bubbling and the fish is browning, indicating that the oil is hot enough to cook the fish.</t>
   </si>
   <si>
-    <t>There are three people in the image, one is a young boy eating pizza, another is a man in a white shirt standing behind him, and the third is a woman sitting at a table in the background.</t>
-  </si>
-  <si>
-    <t>The tree is positioned alongside the railroad tracks, indicating that it is adjacent to the tracks.</t>
-  </si>
-  <si>
     <t>There are two children in the image, each wearing a pair of shorts.</t>
   </si>
   <si>
+    <t>The bike has two wheels, one on the front and one on the back.</t>
+  </si>
+  <si>
     <t>The girl's hair appears to be a shade of brown.</t>
   </si>
   <si>
     <t>The man is positioned on the grass with his feet spread apart, suggesting he is standing.</t>
   </si>
   <si>
-    <t>The machine has lights on and appears to be in use.</t>
-  </si>
-  <si>
-    <t>The shirt appears to be blue in color.</t>
-  </si>
-  <si>
     <t>The ground appears to be covered with grass, which is a common ground cover.</t>
   </si>
   <si>
-    <t>The plate contains a dish with melted cheese, beans, and rice, which are common ingredients in Mexican food.</t>
-  </si>
-  <si>
-    <t>The sign with the red mask contour is typically used to communicate rules or regulations to the public, and in this case, it is indicating that smoking is prohibited in that particular space.</t>
-  </si>
-  <si>
-    <t>The child is surrounded by grass and there are no visible structures or landmarks in the background, indicating an outdoor, open space.</t>
-  </si>
-  <si>
-    <t>The street appears to be wet, likely due to recent rain.</t>
-  </si>
-  <si>
-    <t>The faucet is attached to the sink and is part of the sink's fixtures.</t>
+    <t>The mound's shape and size suggest it has been shaped by natural forces over time, rather than being intentionally constructed by humans.</t>
+  </si>
+  <si>
+    <t>The man's attire is appropriate for a formal or semi-formal event, such as a tennis match or a formal tennis club gathering.</t>
+  </si>
+  <si>
+    <t>The person is wearing skis and poles, and is in a downhill skiing stance on a snowy slope.</t>
+  </si>
+  <si>
+    <t>Snow typically falls from the sky during winter months and accumulates on the ground, creating a layer of snow that can be seen in the image.</t>
+  </si>
+  <si>
+    <t>There are three distinct peaks visible in the background, which are characteristic of mountain ranges.</t>
   </si>
   <si>
     <t>The umbrella is open and being held above the girl's head.</t>
   </si>
   <si>
-    <t>The pot is placed on the step, which is part of the staircase.</t>
-  </si>
-  <si>
-    <t>The man is holding a device that resembles a video game controller, which is commonly used to interact with video games.</t>
+    <t>The train car has a predominantly green color with some red and white accents.</t>
+  </si>
+  <si>
+    <t>The carrots on the table come in various sizes and colors, indicating a variety.</t>
   </si>
   <si>
     <t>There are three magazines stacked on the table.</t>
   </si>
   <si>
-    <t>The spoon is partially submerged in the pot of rice, indicating it is being used to stir the rice.</t>
-  </si>
-  <si>
-    <t>The cars of the train are painted in a bright blue color, which is a common color for train cars.</t>
+    <t>There are two players on the tennis court, one serving and one receiving.</t>
+  </si>
+  <si>
+    <t>There is only one person visible on the motorcycle.</t>
   </si>
 </sst>
 </file>
@@ -1796,7 +2264,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1842,19 +2310,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
         <v>75</v>
       </c>
       <c r="J2" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="K2" t="s">
-        <v>139</v>
+        <v>204</v>
       </c>
       <c r="L2" t="s">
-        <v>171</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1862,19 +2330,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="I3" t="s">
         <v>76</v>
       </c>
       <c r="J3" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="K3" t="s">
-        <v>140</v>
+        <v>205</v>
       </c>
       <c r="L3" t="s">
-        <v>172</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1882,19 +2350,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="I4" t="s">
         <v>77</v>
       </c>
       <c r="J4" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="K4" t="s">
-        <v>141</v>
+        <v>206</v>
       </c>
       <c r="L4" t="s">
-        <v>173</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1908,13 +2376,13 @@
         <v>78</v>
       </c>
       <c r="J5" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="K5" t="s">
-        <v>139</v>
+        <v>207</v>
       </c>
       <c r="L5" t="s">
-        <v>174</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1922,19 +2390,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="I6" t="s">
         <v>79</v>
       </c>
       <c r="J6" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="K6" t="s">
-        <v>142</v>
+        <v>208</v>
       </c>
       <c r="L6" t="s">
-        <v>175</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1942,19 +2410,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="I7" t="s">
         <v>80</v>
       </c>
       <c r="J7" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="K7" t="s">
-        <v>143</v>
+        <v>209</v>
       </c>
       <c r="L7" t="s">
-        <v>176</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1962,19 +2430,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I8" t="s">
         <v>81</v>
       </c>
       <c r="J8" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="K8" t="s">
-        <v>144</v>
+        <v>210</v>
       </c>
       <c r="L8" t="s">
-        <v>177</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1982,19 +2450,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="I9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J9" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="K9" t="s">
-        <v>145</v>
+        <v>211</v>
       </c>
       <c r="L9" t="s">
-        <v>178</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -2002,19 +2470,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="I10" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="J10" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="K10" t="s">
-        <v>146</v>
+        <v>212</v>
       </c>
       <c r="L10" t="s">
-        <v>179</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2022,19 +2490,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J11" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="K11" t="s">
-        <v>147</v>
+        <v>207</v>
       </c>
       <c r="L11" t="s">
-        <v>180</v>
+        <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2042,19 +2510,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="J12" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="K12" t="s">
-        <v>148</v>
+        <v>207</v>
       </c>
       <c r="L12" t="s">
-        <v>181</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2062,19 +2530,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J13" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="K13" t="s">
-        <v>149</v>
+        <v>213</v>
       </c>
       <c r="L13" t="s">
-        <v>182</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2082,19 +2550,19 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="I14" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J14" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="K14" t="s">
-        <v>145</v>
+        <v>214</v>
       </c>
       <c r="L14" t="s">
-        <v>183</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2102,19 +2570,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="I15" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="J15" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="K15" t="s">
-        <v>150</v>
+        <v>215</v>
       </c>
       <c r="L15" t="s">
-        <v>184</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2122,19 +2590,19 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="J16" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="K16" t="s">
-        <v>139</v>
+        <v>216</v>
       </c>
       <c r="L16" t="s">
-        <v>185</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2142,19 +2610,19 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I17" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="J17" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="K17" t="s">
-        <v>151</v>
+        <v>217</v>
       </c>
       <c r="L17" t="s">
-        <v>186</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -2162,19 +2630,19 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="I18" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="J18" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="K18" t="s">
-        <v>152</v>
+        <v>218</v>
       </c>
       <c r="L18" t="s">
-        <v>187</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -2182,19 +2650,19 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="I19" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="J19" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="K19" t="s">
-        <v>152</v>
+        <v>219</v>
       </c>
       <c r="L19" t="s">
-        <v>188</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -2202,19 +2670,19 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="J20" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="K20" t="s">
-        <v>153</v>
+        <v>220</v>
       </c>
       <c r="L20" t="s">
-        <v>189</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -2222,19 +2690,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="I21" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="J21" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="K21" t="s">
-        <v>154</v>
+        <v>207</v>
       </c>
       <c r="L21" t="s">
-        <v>190</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -2242,19 +2710,19 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="I22" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="J22" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="K22" t="s">
-        <v>155</v>
+        <v>221</v>
       </c>
       <c r="L22" t="s">
-        <v>191</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2262,19 +2730,19 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="I23" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="J23" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="K23" t="s">
-        <v>156</v>
+        <v>222</v>
       </c>
       <c r="L23" t="s">
-        <v>192</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2282,19 +2750,19 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I24" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="J24" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="K24" t="s">
-        <v>157</v>
+        <v>223</v>
       </c>
       <c r="L24" t="s">
-        <v>193</v>
+        <v>299</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2302,19 +2770,19 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I25" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="J25" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="K25" t="s">
-        <v>158</v>
+        <v>224</v>
       </c>
       <c r="L25" t="s">
-        <v>194</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2322,19 +2790,19 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="I26" t="s">
         <v>77</v>
       </c>
       <c r="J26" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="K26" t="s">
-        <v>139</v>
+        <v>225</v>
       </c>
       <c r="L26" t="s">
-        <v>195</v>
+        <v>301</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2342,19 +2810,19 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I27" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="J27" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="K27" t="s">
-        <v>139</v>
+        <v>226</v>
       </c>
       <c r="L27" t="s">
-        <v>196</v>
+        <v>302</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2362,19 +2830,19 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I28" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="J28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K28" t="s">
-        <v>159</v>
+        <v>209</v>
       </c>
       <c r="L28" t="s">
-        <v>197</v>
+        <v>303</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -2382,19 +2850,19 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="I29" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="J29" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="K29" t="s">
-        <v>160</v>
+        <v>213</v>
       </c>
       <c r="L29" t="s">
-        <v>198</v>
+        <v>304</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2402,19 +2870,19 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="I30" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J30" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="K30" t="s">
-        <v>161</v>
+        <v>227</v>
       </c>
       <c r="L30" t="s">
-        <v>199</v>
+        <v>305</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2422,19 +2890,19 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="I31" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="J31" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="K31" t="s">
-        <v>162</v>
+        <v>228</v>
       </c>
       <c r="L31" t="s">
-        <v>200</v>
+        <v>306</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2442,19 +2910,19 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="I32" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="J32" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="K32" t="s">
-        <v>163</v>
+        <v>227</v>
       </c>
       <c r="L32" t="s">
-        <v>201</v>
+        <v>307</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2462,19 +2930,19 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="I33" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="J33" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="K33" t="s">
-        <v>155</v>
+        <v>229</v>
       </c>
       <c r="L33" t="s">
-        <v>202</v>
+        <v>308</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2482,19 +2950,19 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="I34" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="J34" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="K34" t="s">
-        <v>164</v>
+        <v>225</v>
       </c>
       <c r="L34" t="s">
-        <v>203</v>
+        <v>309</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2502,19 +2970,19 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="I35" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="J35" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K35" t="s">
-        <v>152</v>
+        <v>207</v>
       </c>
       <c r="L35" t="s">
-        <v>204</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2522,19 +2990,19 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="I36" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="J36" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="K36" t="s">
-        <v>150</v>
+        <v>230</v>
       </c>
       <c r="L36" t="s">
-        <v>205</v>
+        <v>311</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2542,19 +3010,19 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I37" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J37" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="K37" t="s">
-        <v>165</v>
+        <v>231</v>
       </c>
       <c r="L37" t="s">
-        <v>206</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2562,19 +3030,19 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="I38" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="J38" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="K38" t="s">
-        <v>139</v>
+        <v>232</v>
       </c>
       <c r="L38" t="s">
-        <v>207</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2582,19 +3050,19 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="I39" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="J39" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="K39" t="s">
-        <v>166</v>
+        <v>233</v>
       </c>
       <c r="L39" t="s">
-        <v>208</v>
+        <v>314</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2602,19 +3070,19 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="I40" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J40" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="K40" t="s">
-        <v>139</v>
+        <v>234</v>
       </c>
       <c r="L40" t="s">
-        <v>209</v>
+        <v>315</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2622,19 +3090,19 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="I41" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="J41" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="K41" t="s">
-        <v>140</v>
+        <v>235</v>
       </c>
       <c r="L41" t="s">
-        <v>210</v>
+        <v>316</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2642,19 +3110,19 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="I42" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="J42" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="K42" t="s">
-        <v>167</v>
+        <v>207</v>
       </c>
       <c r="L42" t="s">
-        <v>211</v>
+        <v>317</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2662,19 +3130,19 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="I43" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J43" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="K43" t="s">
-        <v>168</v>
+        <v>236</v>
       </c>
       <c r="L43" t="s">
-        <v>212</v>
+        <v>318</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2682,19 +3150,19 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="I44" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="J44" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="K44" t="s">
-        <v>139</v>
+        <v>207</v>
       </c>
       <c r="L44" t="s">
-        <v>213</v>
+        <v>319</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2702,19 +3170,19 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="I45" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="J45" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="K45" t="s">
-        <v>139</v>
+        <v>237</v>
       </c>
       <c r="L45" t="s">
-        <v>214</v>
+        <v>320</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2722,19 +3190,19 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="I46" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="J46" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="K46" t="s">
-        <v>139</v>
+        <v>238</v>
       </c>
       <c r="L46" t="s">
-        <v>215</v>
+        <v>321</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2742,19 +3210,19 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I47" t="s">
         <v>85</v>
       </c>
       <c r="J47" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="K47" t="s">
-        <v>139</v>
+        <v>239</v>
       </c>
       <c r="L47" t="s">
-        <v>216</v>
+        <v>322</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -2762,19 +3230,19 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="I48" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="J48" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="K48" t="s">
-        <v>169</v>
+        <v>240</v>
       </c>
       <c r="L48" t="s">
-        <v>217</v>
+        <v>323</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -2782,19 +3250,19 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="I49" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="J49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K49" t="s">
-        <v>155</v>
+        <v>225</v>
       </c>
       <c r="L49" t="s">
-        <v>218</v>
+        <v>324</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -2802,19 +3270,19 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="I50" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="J50" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="K50" t="s">
-        <v>139</v>
+        <v>241</v>
       </c>
       <c r="L50" t="s">
-        <v>219</v>
+        <v>325</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -2822,19 +3290,1019 @@
         <v>49</v>
       </c>
       <c r="B51">
+        <v>14</v>
+      </c>
+      <c r="I51" t="s">
+        <v>92</v>
+      </c>
+      <c r="J51" t="s">
+        <v>155</v>
+      </c>
+      <c r="K51" t="s">
+        <v>207</v>
+      </c>
+      <c r="L51" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>25</v>
+      </c>
+      <c r="I52" t="s">
+        <v>94</v>
+      </c>
+      <c r="J52" t="s">
+        <v>156</v>
+      </c>
+      <c r="K52" t="s">
+        <v>242</v>
+      </c>
+      <c r="L52" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="I53" t="s">
+        <v>90</v>
+      </c>
+      <c r="J53" t="s">
+        <v>157</v>
+      </c>
+      <c r="K53" t="s">
+        <v>207</v>
+      </c>
+      <c r="L53" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>18</v>
+      </c>
+      <c r="I54" t="s">
+        <v>95</v>
+      </c>
+      <c r="J54" t="s">
+        <v>158</v>
+      </c>
+      <c r="K54" t="s">
+        <v>243</v>
+      </c>
+      <c r="L54" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
         <v>39</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I55" t="s">
+        <v>105</v>
+      </c>
+      <c r="J55" t="s">
+        <v>159</v>
+      </c>
+      <c r="K55" t="s">
+        <v>244</v>
+      </c>
+      <c r="L55" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>9</v>
+      </c>
+      <c r="I56" t="s">
+        <v>103</v>
+      </c>
+      <c r="J56" t="s">
+        <v>160</v>
+      </c>
+      <c r="K56" t="s">
+        <v>245</v>
+      </c>
+      <c r="L56" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>79</v>
+      </c>
+      <c r="I57" t="s">
+        <v>91</v>
+      </c>
+      <c r="J57" t="s">
+        <v>161</v>
+      </c>
+      <c r="K57" t="s">
+        <v>246</v>
+      </c>
+      <c r="L57" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>7</v>
+      </c>
+      <c r="I58" t="s">
+        <v>103</v>
+      </c>
+      <c r="J58" t="s">
+        <v>162</v>
+      </c>
+      <c r="K58" t="s">
+        <v>247</v>
+      </c>
+      <c r="L58" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>65</v>
+      </c>
+      <c r="I59" t="s">
+        <v>101</v>
+      </c>
+      <c r="J59" t="s">
+        <v>163</v>
+      </c>
+      <c r="K59" t="s">
+        <v>248</v>
+      </c>
+      <c r="L59" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>37</v>
+      </c>
+      <c r="I60" t="s">
+        <v>105</v>
+      </c>
+      <c r="J60" t="s">
+        <v>164</v>
+      </c>
+      <c r="K60" t="s">
+        <v>249</v>
+      </c>
+      <c r="L60" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>90</v>
+      </c>
+      <c r="I61" t="s">
+        <v>89</v>
+      </c>
+      <c r="J61" t="s">
+        <v>165</v>
+      </c>
+      <c r="K61" t="s">
+        <v>250</v>
+      </c>
+      <c r="L61" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>57</v>
+      </c>
+      <c r="I62" t="s">
+        <v>93</v>
+      </c>
+      <c r="J62" t="s">
+        <v>130</v>
+      </c>
+      <c r="K62" t="s">
+        <v>251</v>
+      </c>
+      <c r="L62" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>100</v>
+      </c>
+      <c r="I63" t="s">
+        <v>106</v>
+      </c>
+      <c r="J63" t="s">
+        <v>166</v>
+      </c>
+      <c r="K63" t="s">
+        <v>213</v>
+      </c>
+      <c r="L63" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>55</v>
+      </c>
+      <c r="I64" t="s">
+        <v>93</v>
+      </c>
+      <c r="J64" t="s">
+        <v>167</v>
+      </c>
+      <c r="K64" t="s">
+        <v>252</v>
+      </c>
+      <c r="L64" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>44</v>
+      </c>
+      <c r="I65" t="s">
+        <v>79</v>
+      </c>
+      <c r="J65" t="s">
+        <v>168</v>
+      </c>
+      <c r="K65" t="s">
+        <v>207</v>
+      </c>
+      <c r="L65" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>51</v>
+      </c>
+      <c r="I66" t="s">
+        <v>102</v>
+      </c>
+      <c r="J66" t="s">
+        <v>169</v>
+      </c>
+      <c r="K66" t="s">
+        <v>253</v>
+      </c>
+      <c r="L66" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>68</v>
+      </c>
+      <c r="I67" t="s">
+        <v>100</v>
+      </c>
+      <c r="J67" t="s">
+        <v>170</v>
+      </c>
+      <c r="K67" t="s">
+        <v>254</v>
+      </c>
+      <c r="L67" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>47</v>
+      </c>
+      <c r="I68" t="s">
+        <v>78</v>
+      </c>
+      <c r="J68" t="s">
+        <v>171</v>
+      </c>
+      <c r="K68" t="s">
+        <v>232</v>
+      </c>
+      <c r="L68" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>69</v>
+      </c>
+      <c r="I69" t="s">
+        <v>77</v>
+      </c>
+      <c r="J69" t="s">
+        <v>172</v>
+      </c>
+      <c r="K69" t="s">
+        <v>255</v>
+      </c>
+      <c r="L69" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>62</v>
+      </c>
+      <c r="I70" t="s">
+        <v>104</v>
+      </c>
+      <c r="J70" t="s">
+        <v>173</v>
+      </c>
+      <c r="K70" t="s">
+        <v>256</v>
+      </c>
+      <c r="L70" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>98</v>
+      </c>
+      <c r="I71" t="s">
+        <v>106</v>
+      </c>
+      <c r="J71" t="s">
+        <v>174</v>
+      </c>
+      <c r="K71" t="s">
+        <v>257</v>
+      </c>
+      <c r="L71" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>80</v>
+      </c>
+      <c r="I72" t="s">
+        <v>82</v>
+      </c>
+      <c r="J72" t="s">
+        <v>175</v>
+      </c>
+      <c r="K72" t="s">
+        <v>258</v>
+      </c>
+      <c r="L72" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>42</v>
+      </c>
+      <c r="I73" t="s">
+        <v>80</v>
+      </c>
+      <c r="J73" t="s">
+        <v>176</v>
+      </c>
+      <c r="K73" t="s">
+        <v>232</v>
+      </c>
+      <c r="L73" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>59</v>
+      </c>
+      <c r="I74" t="s">
+        <v>107</v>
+      </c>
+      <c r="J74" t="s">
+        <v>177</v>
+      </c>
+      <c r="K74" t="s">
+        <v>259</v>
+      </c>
+      <c r="L74" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>49</v>
+      </c>
+      <c r="I75" t="s">
+        <v>102</v>
+      </c>
+      <c r="J75" t="s">
+        <v>178</v>
+      </c>
+      <c r="K75" t="s">
+        <v>260</v>
+      </c>
+      <c r="L75" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>99</v>
+      </c>
+      <c r="I76" t="s">
+        <v>106</v>
+      </c>
+      <c r="J76" t="s">
+        <v>179</v>
+      </c>
+      <c r="K76" t="s">
+        <v>261</v>
+      </c>
+      <c r="L76" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>58</v>
+      </c>
+      <c r="I77" t="s">
+        <v>107</v>
+      </c>
+      <c r="J77" t="s">
+        <v>180</v>
+      </c>
+      <c r="K77" t="s">
+        <v>262</v>
+      </c>
+      <c r="L77" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>76</v>
+      </c>
+      <c r="I78" t="s">
+        <v>108</v>
+      </c>
+      <c r="J78" t="s">
+        <v>181</v>
+      </c>
+      <c r="K78" t="s">
+        <v>263</v>
+      </c>
+      <c r="L78" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>33</v>
+      </c>
+      <c r="I79" t="s">
+        <v>86</v>
+      </c>
+      <c r="J79" t="s">
+        <v>182</v>
+      </c>
+      <c r="K79" t="s">
+        <v>264</v>
+      </c>
+      <c r="L79" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>95</v>
+      </c>
+      <c r="I80" t="s">
+        <v>96</v>
+      </c>
+      <c r="J80" t="s">
+        <v>183</v>
+      </c>
+      <c r="K80" t="s">
+        <v>265</v>
+      </c>
+      <c r="L80" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>60</v>
+      </c>
+      <c r="I81" t="s">
+        <v>107</v>
+      </c>
+      <c r="J81" t="s">
+        <v>184</v>
+      </c>
+      <c r="K81" t="s">
+        <v>266</v>
+      </c>
+      <c r="L81" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>64</v>
+      </c>
+      <c r="I82" t="s">
+        <v>101</v>
+      </c>
+      <c r="J82" t="s">
+        <v>185</v>
+      </c>
+      <c r="K82" t="s">
+        <v>267</v>
+      </c>
+      <c r="L82" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>85</v>
+      </c>
+      <c r="I83" t="s">
+        <v>75</v>
+      </c>
+      <c r="J83" t="s">
+        <v>186</v>
+      </c>
+      <c r="K83" t="s">
+        <v>268</v>
+      </c>
+      <c r="L83" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>38</v>
+      </c>
+      <c r="I84" t="s">
+        <v>105</v>
+      </c>
+      <c r="J84" t="s">
+        <v>134</v>
+      </c>
+      <c r="K84" t="s">
+        <v>225</v>
+      </c>
+      <c r="L84" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>30</v>
+      </c>
+      <c r="I85" t="s">
+        <v>98</v>
+      </c>
+      <c r="J85" t="s">
+        <v>187</v>
+      </c>
+      <c r="K85" t="s">
+        <v>269</v>
+      </c>
+      <c r="L85" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86" s="1">
         <v>84</v>
       </c>
-      <c r="J51" t="s">
-        <v>138</v>
-      </c>
-      <c r="K51" t="s">
-        <v>170</v>
-      </c>
-      <c r="L51" t="s">
-        <v>220</v>
+      <c r="B86">
+        <v>2</v>
+      </c>
+      <c r="I86" t="s">
+        <v>84</v>
+      </c>
+      <c r="J86" t="s">
+        <v>188</v>
+      </c>
+      <c r="K86" t="s">
+        <v>232</v>
+      </c>
+      <c r="L86" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>53</v>
+      </c>
+      <c r="I87" t="s">
+        <v>76</v>
+      </c>
+      <c r="J87" t="s">
+        <v>189</v>
+      </c>
+      <c r="K87" t="s">
+        <v>232</v>
+      </c>
+      <c r="L87" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>22</v>
+      </c>
+      <c r="I88" t="s">
+        <v>81</v>
+      </c>
+      <c r="J88" t="s">
+        <v>190</v>
+      </c>
+      <c r="K88" t="s">
+        <v>245</v>
+      </c>
+      <c r="L88" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>3</v>
+      </c>
+      <c r="I89" t="s">
+        <v>84</v>
+      </c>
+      <c r="J89" t="s">
+        <v>191</v>
+      </c>
+      <c r="K89" t="s">
+        <v>270</v>
+      </c>
+      <c r="L89" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>24</v>
+      </c>
+      <c r="I90" t="s">
+        <v>81</v>
+      </c>
+      <c r="J90" t="s">
+        <v>192</v>
+      </c>
+      <c r="K90" t="s">
+        <v>207</v>
+      </c>
+      <c r="L90" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>88</v>
+      </c>
+      <c r="I91" t="s">
+        <v>97</v>
+      </c>
+      <c r="J91" t="s">
+        <v>193</v>
+      </c>
+      <c r="K91" t="s">
+        <v>271</v>
+      </c>
+      <c r="L91" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>92</v>
+      </c>
+      <c r="I92" t="s">
+        <v>99</v>
+      </c>
+      <c r="J92" t="s">
+        <v>194</v>
+      </c>
+      <c r="K92" t="s">
+        <v>272</v>
+      </c>
+      <c r="L92" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>75</v>
+      </c>
+      <c r="I93" t="s">
+        <v>108</v>
+      </c>
+      <c r="J93" t="s">
+        <v>195</v>
+      </c>
+      <c r="K93" t="s">
+        <v>273</v>
+      </c>
+      <c r="L93" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>87</v>
+      </c>
+      <c r="I94" t="s">
+        <v>97</v>
+      </c>
+      <c r="J94" t="s">
+        <v>196</v>
+      </c>
+      <c r="K94" t="s">
+        <v>274</v>
+      </c>
+      <c r="L94" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>83</v>
+      </c>
+      <c r="I95" t="s">
+        <v>75</v>
+      </c>
+      <c r="J95" t="s">
+        <v>197</v>
+      </c>
+      <c r="K95" t="s">
+        <v>227</v>
+      </c>
+      <c r="L95" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>21</v>
+      </c>
+      <c r="I96" t="s">
+        <v>85</v>
+      </c>
+      <c r="J96" t="s">
+        <v>198</v>
+      </c>
+      <c r="K96" t="s">
+        <v>207</v>
+      </c>
+      <c r="L96" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>61</v>
+      </c>
+      <c r="I97" t="s">
+        <v>104</v>
+      </c>
+      <c r="J97" t="s">
+        <v>199</v>
+      </c>
+      <c r="K97" t="s">
+        <v>275</v>
+      </c>
+      <c r="L97" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>72</v>
+      </c>
+      <c r="I98" t="s">
+        <v>109</v>
+      </c>
+      <c r="J98" t="s">
+        <v>200</v>
+      </c>
+      <c r="K98" t="s">
+        <v>276</v>
+      </c>
+      <c r="L98" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>15</v>
+      </c>
+      <c r="I99" t="s">
+        <v>92</v>
+      </c>
+      <c r="J99" t="s">
+        <v>201</v>
+      </c>
+      <c r="K99" t="s">
+        <v>227</v>
+      </c>
+      <c r="L99" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>93</v>
+      </c>
+      <c r="I100" t="s">
+        <v>99</v>
+      </c>
+      <c r="J100" t="s">
+        <v>202</v>
+      </c>
+      <c r="K100" t="s">
+        <v>232</v>
+      </c>
+      <c r="L100" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>52</v>
+      </c>
+      <c r="I101" t="s">
+        <v>76</v>
+      </c>
+      <c r="J101" t="s">
+        <v>203</v>
+      </c>
+      <c r="K101" t="s">
+        <v>213</v>
+      </c>
+      <c r="L101" t="s">
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>